<commit_message>
Can now read the first 5 lines of an xlsx file
</commit_message>
<xml_diff>
--- a/PracticeData.xlsx
+++ b/PracticeData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Title</t>
   </si>
@@ -19,7 +19,13 @@
     <t>Id</t>
   </si>
   <si>
+    <t>shape</t>
+  </si>
+  <si>
     <t>Red</t>
+  </si>
+  <si>
+    <t>circle</t>
   </si>
   <si>
     <t>Green</t>
@@ -32,7 +38,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -42,6 +48,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -57,11 +68,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -287,29 +307,74 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
         <v>1.0</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3.0</v>
+      <c r="B5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created basic sqlite db, and created shapes table
</commit_message>
<xml_diff>
--- a/PracticeData.xlsx
+++ b/PracticeData.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>Title</t>
   </si>
@@ -32,6 +33,9 @@
   </si>
   <si>
     <t>Blue</t>
+  </si>
+  <si>
+    <t>color</t>
   </si>
 </sst>
 </file>
@@ -93,6 +97,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -318,7 +326,7 @@
       <c r="B2" s="3">
         <v>1.0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -375,6 +383,98 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>